<commit_message>
model pixel done, sisa downloadable file
</commit_message>
<xml_diff>
--- a/ProDS2/Prediction/klasifikasi_bertahap_5.xlsx
+++ b/ProDS2/Prediction/klasifikasi_bertahap_5.xlsx
@@ -6585,7 +6585,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>tank_road_river</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -6777,7 +6777,7 @@
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -9357,7 +9357,7 @@
       </c>
       <c r="B744" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>tank_road_river</t>
         </is>
       </c>
     </row>
@@ -11613,7 +11613,7 @@
       </c>
       <c r="B932" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>tank_road_river</t>
         </is>
       </c>
     </row>
@@ -12501,7 +12501,7 @@
       </c>
       <c r="B1006" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -14397,7 +14397,7 @@
       </c>
       <c r="B1164" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>

</xml_diff>